<commit_message>
integrate wdg reboot refactor
</commit_message>
<xml_diff>
--- a/docs/hw/meas/ES-MC-210707C - MyOmniscient conso estimation.xlsx
+++ b/docs/hw/meas/ES-MC-210707C - MyOmniscient conso estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\03-Git\exotic\products\my-omniscient\position-switch-connected\proto-rak5010-arduino\docs\hw\meas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C31E6CA-BB85-44C6-A575-FC72DE911B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0D95CA-6435-4253-AB8A-D5065773F93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conso(PERIODIC)" sheetId="1" r:id="rId1"/>
@@ -955,7 +955,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,10 +1032,10 @@
         <v>23</v>
       </c>
       <c r="E3" s="5">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F3" s="7">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>16</v>
@@ -1058,7 +1058,7 @@
         <v>75</v>
       </c>
       <c r="F4" s="7">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
@@ -1152,11 +1152,11 @@
       </c>
       <c r="G17" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité HB]]*$F$3)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="H17" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité Event]]*$F$4)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="I17" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité recharge super cap]]*$F$5)</f>
@@ -1164,19 +1164,19 @@
       </c>
       <c r="J17" s="15">
         <f>Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]-H17-G17-I17</f>
-        <v>23.825000000000003</v>
+        <v>23.786111111111111</v>
       </c>
       <c r="K17" s="27">
         <f>($E$2*Tableau5[[#This Row],[Temps veille /24h]]+$E$3*Tableau5[[#This Row],[Temps GPS /24h]]+$E$4*Tableau5[[#This Row],[Temps émission /24h]]+$E$5*Tableau5[[#This Row],[Temps de recharge super capa /24h]])/24</f>
-        <v>1.5148090277777781</v>
+        <v>1.624311342592593</v>
       </c>
       <c r="L17" s="18">
         <f>$B$4/(Tableau5[[#This Row],[Consommation /24h]]*$B$3)</f>
-        <v>9572.1637078381245</v>
+        <v>8926.8600297134453</v>
       </c>
       <c r="M17" s="19">
         <f>Tableau5[[#This Row],[Autonomie en heure]]/24</f>
-        <v>398.84015449325517</v>
+        <v>371.95250123806022</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1203,11 +1203,11 @@
       </c>
       <c r="G18" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité HB]]*$F$3)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="H18" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité Event]]*$F$4)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="I18" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité recharge super cap]]*$F$5)</f>
@@ -1215,19 +1215,19 @@
       </c>
       <c r="J18" s="15">
         <f>Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]-H18-G18-I18</f>
-        <v>23.737500000000001</v>
+        <v>23.686111111111114</v>
       </c>
       <c r="K18" s="27">
         <f>($E$2*Tableau5[[#This Row],[Temps veille /24h]]+$E$3*Tableau5[[#This Row],[Temps GPS /24h]]+$E$4*Tableau5[[#This Row],[Temps émission /24h]]+$E$5*Tableau5[[#This Row],[Temps de recharge super capa /24h]])/24</f>
-        <v>1.5972135416666668</v>
+        <v>1.7450752314814817</v>
       </c>
       <c r="L18" s="18">
         <f>$B$4/(Tableau5[[#This Row],[Consommation /24h]]*$B$3)</f>
-        <v>9078.3102082076512</v>
+        <v>8309.0973606279567</v>
       </c>
       <c r="M18" s="19">
         <f>Tableau5[[#This Row],[Autonomie en heure]]/24</f>
-        <v>378.26292534198546</v>
+        <v>346.21239002616488</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1254,11 +1254,11 @@
       </c>
       <c r="G19" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité HB]]*$F$3)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="H19" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité Event]]*$F$4)</f>
-        <v>6.25E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I19" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité recharge super cap]]*$F$5)</f>
@@ -1266,19 +1266,19 @@
       </c>
       <c r="J19" s="15">
         <f>Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]-H19-G19-I19</f>
-        <v>23.650000000000002</v>
+        <v>23.586111111111112</v>
       </c>
       <c r="K19" s="28">
         <f>($E$2*Tableau5[[#This Row],[Temps veille /24h]]+$E$3*Tableau5[[#This Row],[Temps GPS /24h]]+$E$4*Tableau5[[#This Row],[Temps émission /24h]]+$E$5*Tableau5[[#This Row],[Temps de recharge super capa /24h]])/24</f>
-        <v>1.679618055555556</v>
+        <v>1.8658391203703706</v>
       </c>
       <c r="L19" s="24">
         <f>$B$4/(Tableau5[[#This Row],[Consommation /24h]]*$B$3)</f>
-        <v>8632.9150559196223</v>
+        <v>7771.302381698235</v>
       </c>
       <c r="M19" s="25">
         <f>Tableau5[[#This Row],[Autonomie en heure]]/24</f>
-        <v>359.70479399665095</v>
+        <v>323.80426590409314</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1305,11 +1305,11 @@
       </c>
       <c r="G20" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité HB]]*$F$3)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="H20" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité Event]]*$F$4)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="I20" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité recharge super cap]]*$F$5)</f>
@@ -1317,19 +1317,19 @@
       </c>
       <c r="J20" s="15">
         <f>Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]-H20-G20-I20</f>
-        <v>23.562500000000004</v>
+        <v>23.486111111111114</v>
       </c>
       <c r="K20" s="27">
         <f>($E$2*Tableau5[[#This Row],[Temps veille /24h]]+$E$3*Tableau5[[#This Row],[Temps GPS /24h]]+$E$4*Tableau5[[#This Row],[Temps émission /24h]]+$E$5*Tableau5[[#This Row],[Temps de recharge super capa /24h]])/24</f>
-        <v>1.7620225694444445</v>
+        <v>1.9866030092592595</v>
       </c>
       <c r="L20" s="18">
         <f>$B$4/(Tableau5[[#This Row],[Consommation /24h]]*$B$3)</f>
-        <v>8229.179496021874</v>
+        <v>7298.8915915347297</v>
       </c>
       <c r="M20" s="19">
         <f>Tableau5[[#This Row],[Autonomie en heure]]/24</f>
-        <v>342.88247900091142</v>
+        <v>304.12048298061376</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="26">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C21" s="13">
         <v>24</v>
@@ -1348,39 +1348,39 @@
       </c>
       <c r="E21" s="14">
         <f>86400/Tableau5[[#This Row],[Nb d''event /24h]]</f>
-        <v>1234.2857142857142</v>
+        <v>2160</v>
       </c>
       <c r="F21" s="14">
         <f>86400/(Tableau5[[#This Row],[Nb de HB /24h]]+Tableau5[[#This Row],[Nb d''event /24h]])</f>
-        <v>1216.9014084507041</v>
+        <v>2107.3170731707319</v>
       </c>
       <c r="G21" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité HB]]*$F$3)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="H21" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité Event]]*$F$4)</f>
-        <v>1.4583333333333333</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="I21" s="15">
         <f>(Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]/Tableau5[[#This Row],[Périodicité recharge super cap]]*$F$5)</f>
-        <v>4.7333333333333343</v>
+        <v>2.7333333333333329</v>
       </c>
       <c r="J21" s="15">
         <f>Tableau5[[#This Row],[Nb d''heures d''utilisation /24h]]-H21-G21-I21</f>
-        <v>17.787500000000001</v>
+        <v>19.886111111111113</v>
       </c>
       <c r="K21" s="27">
         <f>($E$2*Tableau5[[#This Row],[Temps veille /24h]]+$E$3*Tableau5[[#This Row],[Temps GPS /24h]]+$E$4*Tableau5[[#This Row],[Temps émission /24h]]+$E$5*Tableau5[[#This Row],[Temps de recharge super capa /24h]])/24</f>
-        <v>7.2007204861111118</v>
+        <v>6.3341030092592598</v>
       </c>
       <c r="L21" s="18">
         <f>$B$4/(Tableau5[[#This Row],[Consommation /24h]]*$B$3)</f>
-        <v>2013.6873841954953</v>
+        <v>2289.1954833705331</v>
       </c>
       <c r="M21" s="19">
         <f>Tableau5[[#This Row],[Autonomie en heure]]/24</f>
-        <v>83.903641008145641</v>
+        <v>95.383145140438884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>